<commit_message>
Species variability information included in methods, results and figures
</commit_message>
<xml_diff>
--- a/results/Supplementary/2. Results incubator models fixed factors.xlsx
+++ b/results/Supplementary/2. Results incubator models fixed factors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -503,6 +503,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,59 +560,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,10 +581,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,44 +895,44 @@
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="23"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
@@ -969,13 +965,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="6">
         <v>0.32779999999999998</v>
       </c>
@@ -1008,11 +1004,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="9">
         <v>-1.3129999999999999</v>
       </c>
@@ -1045,13 +1041,13 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="6">
         <v>-8.9130000000000003</v>
       </c>
@@ -1084,11 +1080,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="9">
         <v>5.2750000000000004</v>
       </c>
@@ -1121,13 +1117,13 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="6">
         <v>-4.0134999999999996</v>
       </c>
@@ -1160,11 +1156,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="29"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="9">
         <v>-1.482</v>
       </c>
@@ -1197,13 +1193,13 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="6">
         <v>-6.18</v>
       </c>
@@ -1236,11 +1232,11 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="9">
         <v>1.8939999999999999</v>
       </c>
@@ -1273,13 +1269,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="6">
         <v>4.3683300000000003</v>
       </c>
@@ -1312,11 +1308,11 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="9">
         <v>-0.18778</v>
       </c>
@@ -1349,13 +1345,13 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="6">
         <v>-1.6990000000000002E-2</v>
       </c>
@@ -1388,11 +1384,11 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="9">
         <v>0.33189999999999997</v>
       </c>
@@ -1425,13 +1421,13 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="6">
         <v>0.14607000000000001</v>
       </c>
@@ -1464,11 +1460,11 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="34" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="3">
         <v>-0.16617999999999999</v>
       </c>
@@ -1502,6 +1498,23 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -1511,23 +1524,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:M3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>